<commit_message>
filter for trademark cost calc
</commit_message>
<xml_diff>
--- a/nft_stats.xlsx
+++ b/nft_stats.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -609,7 +609,7 @@
         <v>20</v>
       </c>
       <c r="N3" t="str">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O3" t="str">
         <v>2</v>
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="S3" t="str">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T3" t="str">
         <v>3</v>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="str">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y3" t="str">
         <v>8</v>
@@ -2256,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="N24" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O24" t="str">
         <v>0</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>0xfe01e368d65504d620b2d89f987232400210a5fb</v>
+        <v>0xa4ada63fa9417e00c2794cd51db7e9a6aaa473d9</v>
       </c>
       <c r="B42" t="str">
         <v>3</v>
@@ -3624,34 +3624,34 @@
         <v>0</v>
       </c>
       <c r="D42" t="str">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E42" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G42" t="str">
         <v>0.00</v>
       </c>
       <c r="H42" t="str">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I42" t="str">
         <v>0</v>
       </c>
       <c r="J42" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="str">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="L42" t="str">
-        <v>0.40</v>
+        <v>3.11</v>
       </c>
       <c r="M42" t="str">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N42" t="str">
         <v>0</v>
@@ -3660,13 +3660,13 @@
         <v>0</v>
       </c>
       <c r="P42" t="str">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="Q42" t="str">
-        <v>0.40</v>
+        <v>3.19</v>
       </c>
       <c r="R42" t="str">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="S42" t="str">
         <v>1</v>
@@ -3675,13 +3675,13 @@
         <v>0</v>
       </c>
       <c r="U42" t="str">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="V42" t="str">
-        <v>0.01</v>
+        <v>0.10</v>
       </c>
       <c r="W42" t="str">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="X42" t="str">
         <v>0</v>
@@ -3690,51 +3690,51 @@
         <v>0</v>
       </c>
       <c r="Z42" t="str">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="AA42" t="str">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>0x31f38a4e6cd69a8f4176537df3fc5db7ab1c2da5</v>
+        <v>0xfe01e368d65504d620b2d89f987232400210a5fb</v>
       </c>
       <c r="B43" t="str">
         <v>3</v>
       </c>
       <c r="C43" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="str">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E43" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="str">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G43" t="str">
-        <v>0.31</v>
+        <v>0.00</v>
       </c>
       <c r="H43" t="str">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="I43" t="str">
         <v>0</v>
       </c>
       <c r="J43" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="str">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="L43" t="str">
-        <v>2.87</v>
+        <v>0.40</v>
       </c>
       <c r="M43" t="str">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="N43" t="str">
         <v>0</v>
@@ -3743,28 +3743,28 @@
         <v>0</v>
       </c>
       <c r="P43" t="str">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="Q43" t="str">
-        <v>2.91</v>
+        <v>0.40</v>
       </c>
       <c r="R43" t="str">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="S43" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43" t="str">
         <v>0</v>
       </c>
       <c r="U43" t="str">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="V43" t="str">
-        <v>0.08</v>
+        <v>0.01</v>
       </c>
       <c r="W43" t="str">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X43" t="str">
         <v>0</v>
@@ -3773,190 +3773,190 @@
         <v>0</v>
       </c>
       <c r="Z43" t="str">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="AA43" t="str">
-        <v>0.07</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>0xeb9c8b66cab4361801b43eeb1a090f0a3ccd1f5d</v>
+        <v>0x31f38a4e6cd69a8f4176537df3fc5db7ab1c2da5</v>
       </c>
       <c r="B44" t="str">
         <v>3</v>
       </c>
       <c r="C44" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E44" t="str">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="G44" t="str">
-        <v>0.00</v>
+        <v>0.31</v>
       </c>
       <c r="H44" t="str">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I44" t="str">
         <v>0</v>
       </c>
       <c r="J44" t="str">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="K44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L44" t="str">
-        <v>0.00</v>
+        <v>2.87</v>
       </c>
       <c r="M44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="N44" t="str">
         <v>0</v>
       </c>
       <c r="O44" t="str">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="P44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Q44" t="str">
-        <v>0.00</v>
+        <v>2.91</v>
       </c>
       <c r="R44" t="str">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="S44" t="str">
         <v>0</v>
       </c>
       <c r="T44" t="str">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="U44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="V44" t="str">
-        <v>0.00</v>
+        <v>0.08</v>
       </c>
       <c r="W44" t="str">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="X44" t="str">
         <v>0</v>
       </c>
       <c r="Y44" t="str">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="Z44" t="str">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AA44" t="str">
-        <v>0.00</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>0xb862cdd432abe45edace0517aa12c630dd2f9998</v>
+        <v>0xeb9c8b66cab4361801b43eeb1a090f0a3ccd1f5d</v>
       </c>
       <c r="B45" t="str">
         <v>3</v>
       </c>
       <c r="C45" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="str">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F45" t="str">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G45" t="str">
-        <v>1.22</v>
+        <v>0.00</v>
       </c>
       <c r="H45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="str">
         <v>0</v>
       </c>
       <c r="J45" t="str">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="K45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" t="str">
-        <v>0.40</v>
+        <v>0.00</v>
       </c>
       <c r="M45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" t="str">
         <v>0</v>
       </c>
       <c r="O45" t="str">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="P45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="str">
-        <v>0.34</v>
+        <v>0.00</v>
       </c>
       <c r="R45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S45" t="str">
         <v>0</v>
       </c>
       <c r="T45" t="str">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="U45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V45" t="str">
-        <v>0.01</v>
+        <v>0.00</v>
       </c>
       <c r="W45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X45" t="str">
         <v>0</v>
       </c>
       <c r="Y45" t="str">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="Z45" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA45" t="str">
-        <v>0.02</v>
+        <v>0.00</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>0x561791808a5e499b2704973970243ae38acc7d87</v>
+        <v>0xb862cdd432abe45edace0517aa12c630dd2f9998</v>
       </c>
       <c r="B46" t="str">
         <v>3</v>
       </c>
       <c r="C46" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D46" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" t="str">
         <v>0</v>
@@ -3965,72 +3965,72 @@
         <v>0</v>
       </c>
       <c r="G46" t="str">
-        <v>0.00</v>
+        <v>1.22</v>
       </c>
       <c r="H46" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46" t="str">
         <v>0</v>
       </c>
       <c r="K46" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L46" t="str">
-        <v>0.00</v>
+        <v>0.40</v>
       </c>
       <c r="M46" t="str">
         <v>1</v>
       </c>
       <c r="N46" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O46" t="str">
         <v>0</v>
       </c>
       <c r="P46" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q46" t="str">
-        <v>0.16</v>
+        <v>0.34</v>
       </c>
       <c r="R46" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T46" t="str">
         <v>0</v>
       </c>
       <c r="U46" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V46" t="str">
-        <v>0.00</v>
+        <v>0.01</v>
       </c>
       <c r="W46" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X46" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y46" t="str">
         <v>0</v>
       </c>
       <c r="Z46" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA46" t="str">
-        <v>0.00</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>0xd92f70bbf62a161aff0da63d4f4608094f411eeb</v>
+        <v>0x561791808a5e499b2704973970243ae38acc7d87</v>
       </c>
       <c r="B47" t="str">
         <v>3</v>
@@ -4051,10 +4051,10 @@
         <v>0.00</v>
       </c>
       <c r="H47" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I47" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J47" t="str">
         <v>0</v>
@@ -4063,28 +4063,28 @@
         <v>3</v>
       </c>
       <c r="L47" t="str">
-        <v>0.36</v>
+        <v>0.00</v>
       </c>
       <c r="M47" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N47" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O47" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P47" t="str">
         <v>3</v>
       </c>
       <c r="Q47" t="str">
-        <v>0.00</v>
+        <v>0.16</v>
       </c>
       <c r="R47" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T47" t="str">
         <v>0</v>
@@ -4096,16 +4096,16 @@
         <v>0.00</v>
       </c>
       <c r="W47" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X47" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y47" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z47" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA47" t="str">
         <v>0.00</v>
@@ -4113,126 +4113,126 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>0x13b6cb13d487a7dbfabb18b6c82283e5c65ae7d3</v>
+        <v>0xd92f70bbf62a161aff0da63d4f4608094f411eeb</v>
       </c>
       <c r="B48" t="str">
         <v>3</v>
       </c>
       <c r="C48" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D48" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" t="str">
         <v>0</v>
       </c>
       <c r="F48" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="str">
-        <v>1.53</v>
+        <v>0.00</v>
       </c>
       <c r="H48" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J48" t="str">
         <v>0</v>
       </c>
       <c r="K48" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L48" t="str">
-        <v>0.41</v>
+        <v>0.36</v>
       </c>
       <c r="M48" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" t="str">
         <v>0</v>
       </c>
       <c r="O48" t="str">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P48" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q48" t="str">
-        <v>0.42</v>
+        <v>0.00</v>
       </c>
       <c r="R48" t="str">
         <v>1</v>
       </c>
       <c r="S48" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T48" t="str">
         <v>0</v>
       </c>
       <c r="U48" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V48" t="str">
         <v>0.00</v>
       </c>
       <c r="W48" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X48" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y48" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z48" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA48" t="str">
-        <v>0.01</v>
+        <v>0.00</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>0xfa65e65a6321c37486972d71b3f50400bd43f974</v>
+        <v>0x13b6cb13d487a7dbfabb18b6c82283e5c65ae7d3</v>
       </c>
       <c r="B49" t="str">
         <v>3</v>
       </c>
       <c r="C49" t="str">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D49" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49" t="str">
         <v>0</v>
       </c>
       <c r="F49" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" t="str">
-        <v>0.00</v>
+        <v>1.53</v>
       </c>
       <c r="H49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="str">
         <v>0</v>
       </c>
       <c r="K49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L49" t="str">
-        <v>0.23</v>
+        <v>0.41</v>
       </c>
       <c r="M49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N49" t="str">
         <v>0</v>
@@ -4241,45 +4241,128 @@
         <v>0</v>
       </c>
       <c r="P49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q49" t="str">
-        <v>0.23</v>
+        <v>0.42</v>
       </c>
       <c r="R49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S49" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T49" t="str">
         <v>0</v>
       </c>
       <c r="U49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V49" t="str">
         <v>0.00</v>
       </c>
       <c r="W49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X49" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y49" t="str">
         <v>0</v>
       </c>
       <c r="Z49" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA49" t="str">
         <v>0.01</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>0xfa65e65a6321c37486972d71b3f50400bd43f974</v>
+      </c>
+      <c r="B50" t="str">
+        <v>3</v>
+      </c>
+      <c r="C50" t="str">
+        <v>0</v>
+      </c>
+      <c r="D50" t="str">
+        <v>3</v>
+      </c>
+      <c r="E50" t="str">
+        <v>0</v>
+      </c>
+      <c r="F50" t="str">
+        <v>0</v>
+      </c>
+      <c r="G50" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H50" t="str">
+        <v>2</v>
+      </c>
+      <c r="I50" t="str">
+        <v>1</v>
+      </c>
+      <c r="J50" t="str">
+        <v>0</v>
+      </c>
+      <c r="K50" t="str">
+        <v>2</v>
+      </c>
+      <c r="L50" t="str">
+        <v>0.23</v>
+      </c>
+      <c r="M50" t="str">
+        <v>2</v>
+      </c>
+      <c r="N50" t="str">
+        <v>0</v>
+      </c>
+      <c r="O50" t="str">
+        <v>0</v>
+      </c>
+      <c r="P50" t="str">
+        <v>2</v>
+      </c>
+      <c r="Q50" t="str">
+        <v>0.23</v>
+      </c>
+      <c r="R50" t="str">
+        <v>2</v>
+      </c>
+      <c r="S50" t="str">
+        <v>3</v>
+      </c>
+      <c r="T50" t="str">
+        <v>0</v>
+      </c>
+      <c r="U50" t="str">
+        <v>2</v>
+      </c>
+      <c r="V50" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="W50" t="str">
+        <v>2</v>
+      </c>
+      <c r="X50" t="str">
+        <v>4</v>
+      </c>
+      <c r="Y50" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="str">
+        <v>2</v>
+      </c>
+      <c r="AA50" t="str">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA49"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>